<commit_message>
Template for CCAAU-sand Bay Count KPI changed
</commit_message>
<xml_diff>
--- a/Projects/CCAAU_SAND/Data/template.xlsx
+++ b/Projects/CCAAU_SAND/Data/template.xlsx
@@ -100,7 +100,7 @@
     <t xml:space="preserve">BAY_COUNT_BY_SCENE_TYPE_IN_WHOLE_STORE</t>
   </si>
   <si>
-    <t xml:space="preserve">*</t>
+    <t xml:space="preserve">CCA - STANDARD LONG LANE CHECKOUT,CCA - EXPRESS CHECKOUT,CCA - SELF CHECK OUT,CCA - OTHER - FRONT OF STORE,CCA - INDIES - REST OF STORE,Competitor - STANDARD LONG LANE CHECKOUT,Competitor - EXPRESS CHECKOUT,Competitor - SELF CHECK OUT,Competitor - OTHER - FRONT OF STORE,Competitor - INDIES - REST OF STORE</t>
   </si>
 </sst>
 </file>
@@ -436,11 +436,11 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.280612244898"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.1683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="5.12755102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.59183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.3214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="5.04081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.84183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.3571428571429"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="10.8010204081633"/>
   </cols>
   <sheetData>
@@ -716,12 +716,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4336734693878"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4795918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.719387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.39795918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,12 +827,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.25"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.4387755102041"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
adding assortments kpi in sand
</commit_message>
<xml_diff>
--- a/Projects/CCAAU_SAND/Data/template.xlsx
+++ b/Projects/CCAAU_SAND/Data/template.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Exclude" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Include" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="BayCountKPI" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Assortment" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="31">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -100,7 +101,22 @@
     <t xml:space="preserve">BAY_COUNT_BY_SCENE_TYPE_IN_WHOLE_STORE</t>
   </si>
   <si>
-    <t xml:space="preserve">CCA - STANDARD LONG LANE CHECKOUT,CCA - EXPRESS CHECKOUT,CCA - SELF CHECK OUT,CCA - OTHER - FRONT OF STORE,CCA - INDIES - REST OF STORE,Competitor - STANDARD LONG LANE CHECKOUT,Competitor - EXPRESS CHECKOUT,Competitor - SELF CHECK OUT,Competitor - OTHER - FRONT OF STORE,Competitor - INDIES - REST OF STORE</t>
+    <t xml:space="preserve">CCA 3 Door, CCA - STANDARD LONG LANE CHECKOUT,CCA - EXPRESS CHECKOUT,CCA - SELF CHECK OUT,CCA - OTHER - FRONT OF STORE,CCA - INDIES - REST OF STORE,Competitor - STANDARD LONG LANE CHECKOUT,Competitor - EXPRESS CHECKOUT,Competitor - SELF CHECK OUT,Competitor - OTHER - FRONT OF STORE,Competitor - INDIES - REST OF STORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scene_types_to_exclude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">categories_to_exclude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brands_to_exclude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ean_codes_to_exclude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCA-Standard checkout cooler, 2.2 Pepsi/Schweppes Impulse Cooler</t>
   </si>
 </sst>
 </file>
@@ -279,7 +295,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -345,6 +361,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -434,14 +462,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.59183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="46.3214285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="5.04081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.84183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="45.2244897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -716,12 +744,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.719387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.39795918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.2244897959184"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,13 +854,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.4387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.3877551020408"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,6 +876,56 @@
       </c>
       <c r="B2" s="0" t="s">
         <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.8316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove general cat and brand in assortments
</commit_message>
<xml_diff>
--- a/Projects/CCAAU_SAND/Data/template.xlsx
+++ b/Projects/CCAAU_SAND/Data/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Exclude" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="32">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t xml:space="preserve">CCA-Standard checkout cooler, 2.2 Pepsi/Schweppes Impulse Cooler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General</t>
   </si>
 </sst>
 </file>
@@ -462,14 +465,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="45.2244897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="4.72448979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="44.6836734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -744,11 +747,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,13 +857,14 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="42.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -896,17 +901,16 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.8316326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.1581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="19.4387755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -926,6 +930,12 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>30</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding delt kpi, extra only own manuf
</commit_message>
<xml_diff>
--- a/Projects/CCAAU_SAND/Data/template.xlsx
+++ b/Projects/CCAAU_SAND/Data/template.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="31">
   <si>
     <t xml:space="preserve">KPI</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t xml:space="preserve">CCA-Standard checkout cooler, 2.2 Pepsi/Schweppes Impulse Cooler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General</t>
   </si>
 </sst>
 </file>
@@ -465,14 +462,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="44.6836734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="4.59183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="44.1428571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="4.45408163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -747,12 +744,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.1530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.75"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -863,8 +860,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -907,10 +904,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.1581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.4795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -930,12 +928,6 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>